<commit_message>
Updated for Sprint 1
</commit_message>
<xml_diff>
--- a/docs/logbooks/Ajwoodle - Efforts Logbook.xlsx
+++ b/docs/logbooks/Ajwoodle - Efforts Logbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderwoodle/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderwoodle/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11CD3B1-F1B5-F849-8B4B-6EC2051F7B99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021DCF81-BF17-BB44-B32B-CE3F30E06537}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="24240" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Team Member</t>
   </si>
   <si>
-    <t>Joe, Smith</t>
-  </si>
-  <si>
     <t>Towards objectives</t>
   </si>
   <si>
@@ -158,6 +155,24 @@
   </si>
   <si>
     <t>SkyPi</t>
+  </si>
+  <si>
+    <t>Set up Discord for communication, obtained Rasberry Pi, Installed DietPI OS, configured network settings for SSH, Documentation, SkyPi Mock up for presentation</t>
+  </si>
+  <si>
+    <t>b,c,d,e,f,h,I,j,l,n</t>
+  </si>
+  <si>
+    <t>Attached files, Installed Raspberry Pi OS (can submit ISO if required)</t>
+  </si>
+  <si>
+    <t>Attached files, OS image located on physical devices (Raspberr PI x3)</t>
+  </si>
+  <si>
+    <t>DietPi.txt
+requirements.txt
+SkyPi_2.png
+contributions.png</t>
   </si>
 </sst>
 </file>
@@ -314,11 +329,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -331,14 +345,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,30 +372,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -383,12 +385,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,7 +679,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,210 +695,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22">
+        <v>16</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -905,6 +919,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -912,10 +931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,176 +947,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
     </row>
     <row r="2" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="16"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
-        <v>0</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8">
+    </row>
+    <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="D5" s="8">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8">
-        <v>5</v>
-      </c>
-      <c r="H5" s="8">
-        <v>2</v>
-      </c>
-      <c r="I5" s="8">
-        <v>3</v>
-      </c>
-      <c r="J5" s="8">
-        <v>2</v>
-      </c>
-      <c r="K5" s="8">
-        <v>6</v>
-      </c>
-      <c r="L5" s="8">
-        <v>3</v>
-      </c>
-      <c r="M5" s="8">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8">
-        <v>5</v>
-      </c>
-      <c r="P5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1112,12 +1123,12 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1132,12 +1143,12 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1152,12 +1163,12 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1172,12 +1183,12 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>5</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1192,12 +1203,12 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>6</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1212,12 +1223,12 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1231,26 +1242,6 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>8</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:B2"/>

</xml_diff>

<commit_message>
Sprint #2 - Efforts
</commit_message>
<xml_diff>
--- a/docs/logbooks/Ajwoodle - Efforts Logbook.xlsx
+++ b/docs/logbooks/Ajwoodle - Efforts Logbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderwoodle/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021DCF81-BF17-BB44-B32B-CE3F30E06537}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB1E62A-EDDC-EB45-87D2-20E4C1ECE705}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="24240" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28320" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -173,13 +173,133 @@
 requirements.txt
 SkyPi_2.png
 contributions.png</t>
+  </si>
+  <si>
+    <t>a,b,c,d,e,h,I,m,n</t>
+  </si>
+  <si>
+    <t>Selected new OS for Raspberry Pi's, configured Raspberry Pi's, configured Raspberry Pi SSH key authentication, Testing various sensors on the Raspberry Pi, Testing API's for weather data, soldering electrical components, Raspberry Pi user stories</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">Documentation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">DS18B20 Setup Instructions
+TempWiringDigram.png
+User Stories
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">Python
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Python Modules
+bme280_sensor.py
+darkSky.py
+emailAlert.py
+sensor_and_api.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All files are located on our team's GitHub under the following folders:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Documentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">
+skypi/pi/documents
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Python</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>skypi/pi/py</t>
+    </r>
+  </si>
+  <si>
+    <t>Raspberry Pi images on physical devices
+https://github.com/mblaul/skypi
+Attached file for configuring the BME280 sensor on the Raspberry Pi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -221,6 +341,25 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -329,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -345,6 +484,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -357,21 +523,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -384,16 +535,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -679,36 +824,36 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="42.5" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="8" max="8" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" ht="33" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" ht="41" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -718,13 +863,13 @@
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" ht="24" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
@@ -748,164 +893,181 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:8" ht="68">
+      <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22">
+      <c r="B4" s="10"/>
+      <c r="C4" s="8">
         <v>16</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:8" ht="204">
+      <c r="A5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="9">
+        <v>20</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -919,11 +1081,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -934,10 +1091,10 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -946,29 +1103,29 @@
     <col min="5" max="5" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:16" ht="34" customHeight="1">
+      <c r="A1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-    </row>
-    <row r="2" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+    </row>
+    <row r="2" spans="1:16" ht="41" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -990,27 +1147,27 @@
       <c r="O2" s="12"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
+    <row r="3" spans="1:16" ht="22" customHeight="1">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-    </row>
-    <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+    </row>
+    <row r="4" spans="1:16" ht="24" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1060,7 +1217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="36" customHeight="1">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -1102,27 +1259,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="36" customHeight="1">
       <c r="A6" s="6">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="36" customHeight="1">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -1142,7 +1315,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="36" customHeight="1">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -1162,7 +1335,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="36" customHeight="1">
       <c r="A9" s="6">
         <v>5</v>
       </c>
@@ -1182,7 +1355,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="36" customHeight="1">
       <c r="A10" s="6">
         <v>6</v>
       </c>
@@ -1202,7 +1375,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="36" customHeight="1">
       <c r="A11" s="6">
         <v>7</v>
       </c>
@@ -1222,7 +1395,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="36" customHeight="1">
       <c r="A12" s="6">
         <v>8</v>
       </c>

</xml_diff>